<commit_message>
Unit Process checks for mass balance using check_balance in calculators
</commit_message>
<xml_diff>
--- a/excelData/cementUnits.xlsx
+++ b/excelData/cementUnits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F14D1E-D671-6D41-93B4-933E5E487E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92416670-160E-6A4A-93B5-64A3AB293EB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1260" windowWidth="27640" windowHeight="16540" xr2:uid="{94C69905-85FA-FD47-AACA-486307E1FA4E}"/>
+    <workbookView xWindow="1160" yWindow="1260" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{94C69905-85FA-FD47-AACA-486307E1FA4E}"/>
   </bookViews>
   <sheets>
     <sheet name="c meal mixer" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="MealMixer" localSheetId="0">'c meal mixer'!$A$1:$F$5</definedName>
     <definedName name="MealMixerVar" localSheetId="3">'var meal mixer'!$A$1:$E$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,9 +177,6 @@
     <t>NONE</t>
   </si>
   <si>
-    <t>CaCO3_Meal</t>
-  </si>
-  <si>
     <t>energyFuel</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>flyAsh_fract</t>
+  </si>
+  <si>
+    <t>Meal_CaCO3</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCE611D-9E66-FC4D-9411-2A473C140578}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -690,7 +690,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -710,7 +710,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -763,7 +763,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,7 +852,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -863,7 +863,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -872,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -883,7 +883,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -897,22 +897,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
         <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -978,7 +978,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -993,32 +993,32 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1060,41 +1060,41 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>0.2</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>0.4</v>
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE63004-2FFA-F844-A46D-0BECDBA775CA}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1186,22 +1186,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
         <v>14</v>
@@ -1209,42 +1209,43 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>3.6</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>0.75</v>
       </c>
       <c r="E3">
-        <v>0.8</v>
+        <f>1/'var meal mixer'!C3</f>
+        <v>1.4925373134328357</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1255,19 +1256,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>3.6</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>0.75</v>
       </c>
       <c r="E4">
-        <v>0.8</v>
+        <f>1/'var meal mixer'!C4</f>
+        <v>1.5384615384615383</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1278,19 +1280,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>0.65</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <f>1/'var meal mixer'!C5</f>
+        <v>1.4925373134328357</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1301,19 +1304,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>3.2</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>0.67</v>
       </c>
       <c r="E6">
-        <v>0.8</v>
+        <f>1/'var meal mixer'!C6</f>
+        <v>1.3333333333333333</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1344,29 +1348,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>0.15</v>
@@ -1377,7 +1381,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -1388,7 +1392,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>0.15</v>
@@ -1399,7 +1403,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>0.2</v>

</xml_diff>

<commit_message>
Added calculations for slag in kiln
</commit_message>
<xml_diff>
--- a/excelData/cementUnits.xlsx
+++ b/excelData/cementUnits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5218BF7C-19A5-174B-B61C-2AC7CB823997}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E53850-636D-8D47-AB85-E6FDBEE32120}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1260" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{94C69905-85FA-FD47-AACA-486307E1FA4E}"/>
+    <workbookView xWindow="1160" yWindow="1260" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{94C69905-85FA-FD47-AACA-486307E1FA4E}"/>
   </bookViews>
   <sheets>
     <sheet name="c meal mixer" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="57">
   <si>
     <t>KnownQty</t>
   </si>
@@ -262,6 +262,27 @@
   </si>
   <si>
     <t>Meal_CaCO3</t>
+  </si>
+  <si>
+    <t>2nd Known Substance</t>
+  </si>
+  <si>
+    <t>2Qty Origin</t>
+  </si>
+  <si>
+    <t>clinker_co2</t>
+  </si>
+  <si>
+    <t>Addition</t>
+  </si>
+  <si>
+    <t>slag</t>
+  </si>
+  <si>
+    <t>Subtraction</t>
+  </si>
+  <si>
+    <t>inflow</t>
   </si>
 </sst>
 </file>
@@ -640,7 +661,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA23163-3E52-184E-8C92-A87AA50554C7}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,7 +796,7 @@
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -794,8 +815,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -815,7 +842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -835,7 +862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -855,7 +882,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -875,7 +902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -895,7 +922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -915,7 +942,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -933,6 +960,58 @@
       </c>
       <c r="F8" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1169,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE63004-2FFA-F844-A46D-0BECDBA775CA}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed reversed comubstion eff. calculation bug
</commit_message>
<xml_diff>
--- a/excelData/cementUnits.xlsx
+++ b/excelData/cementUnits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E53850-636D-8D47-AB85-E6FDBEE32120}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDFB9AE-ACF3-AB44-89C0-F204583F115B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1260" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{94C69905-85FA-FD47-AACA-486307E1FA4E}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,16 +924,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>

</xml_diff>